<commit_message>
suite tests + début uml
</commit_message>
<xml_diff>
--- a/Tests.xlsx
+++ b/Tests.xlsx
@@ -12,9 +12,11 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="11078"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="5x5" sheetId="1" r:id="rId1"/>
+    <sheet name="6x6" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="21">
   <si>
     <t>Puzzle 5x5</t>
   </si>
@@ -75,6 +77,18 @@
   </si>
   <si>
     <t>1.7</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> a = 0.05</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> a = 0.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> a = 0.2</t>
+  </si>
+  <si>
+    <t>avg = 15k methode 2</t>
   </si>
 </sst>
 </file>
@@ -244,7 +258,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -288,9 +302,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -301,6 +312,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -318,6 +338,1312 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.14707211638653164"/>
+          <c:y val="5.2491248953556703E-2"/>
+          <c:w val="0.77604161451851195"/>
+          <c:h val="0.68616971493619416"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'5x5'!$C$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v> a = 0.05</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:cat>
+            <c:strRef>
+              <c:f>'5x5'!$B$24:$B$33</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'5x5'!$C$24:$C$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="6">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'5x5'!$D$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v> a = 0.1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:cat>
+            <c:strRef>
+              <c:f>'5x5'!$B$24:$B$33</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'5x5'!$D$24:$D$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="3">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'5x5'!$E$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v> a = 0.2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:cat>
+            <c:strRef>
+              <c:f>'5x5'!$B$24:$B$33</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'5x5'!$E$24:$E$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>63</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:upDownBars>
+          <c:gapWidth val="150"/>
+          <c:upBars>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="15000"/>
+                    <a:lumOff val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:upBars>
+          <c:downBars>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="15000"/>
+                    <a:lumOff val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:downBars>
+        </c:upDownBars>
+        <c:smooth val="0"/>
+        <c:axId val="-1863244864"/>
+        <c:axId val="-1863250848"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-1863244864"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200"/>
+                  <a:t>b</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.92343692333842886"/>
+              <c:y val="0.69246686009012415"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="bg2">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+            <a:tailEnd type="triangle"/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1863250848"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-1863250848"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="80"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR" sz="1000" b="0" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>nombre d'itérations (milliers)</a:t>
+                </a:r>
+                <a:endParaRPr lang="fr-FR" sz="400">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="4.0099146497215729E-2"/>
+              <c:y val="5.249136158348041E-2"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1863244864"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="20"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:legendEntry>
+        <c:idx val="3"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="4"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="5"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="6.5712146842994368E-2"/>
+          <c:y val="0.83681872826616133"/>
+          <c:w val="0.9216242049710629"/>
+          <c:h val="6.1893648647829085E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>254932</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>162487</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>521072</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>56029</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -583,10 +1909,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI19"/>
+  <dimension ref="A1:AI32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -594,7 +1920,7 @@
     <col min="1" max="1" width="12.9296875" style="1" customWidth="1"/>
     <col min="2" max="3" width="9.06640625" style="1"/>
     <col min="4" max="4" width="9.06640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="2.86328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="3.9296875" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="10" width="2.86328125" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="18" width="3.9296875" style="1" bestFit="1" customWidth="1"/>
@@ -609,11 +1935,11 @@
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="18"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="23"/>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.45">
       <c r="B2" s="10" t="s">
@@ -622,11 +1948,11 @@
       <c r="C2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="16"/>
-      <c r="F2" s="17"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="16"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
       <c r="I2" s="12"/>
@@ -1039,11 +2365,11 @@
       </c>
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.45">
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
     </row>
     <row r="11" spans="1:35" x14ac:dyDescent="0.45">
-      <c r="E11" s="20"/>
+      <c r="E11" s="19"/>
     </row>
     <row r="12" spans="1:35" x14ac:dyDescent="0.45">
       <c r="B12" s="3"/>
@@ -1105,7 +2431,7 @@
       <c r="J13" s="1">
         <v>7</v>
       </c>
-      <c r="K13" s="21">
+      <c r="K13" s="20">
         <v>200</v>
       </c>
       <c r="L13" s="1">
@@ -1144,7 +2470,7 @@
       <c r="W13" s="1">
         <v>7</v>
       </c>
-      <c r="X13" s="21">
+      <c r="X13" s="20">
         <v>200</v>
       </c>
     </row>
@@ -1153,6 +2479,9 @@
       <c r="C14" s="6" t="s">
         <v>8</v>
       </c>
+      <c r="D14" s="1">
+        <v>63</v>
+      </c>
     </row>
     <row r="17" spans="2:24" x14ac:dyDescent="0.45">
       <c r="B17" s="3"/>
@@ -1205,7 +2534,7 @@
         <v>15</v>
       </c>
       <c r="D18" s="1">
-        <f t="shared" ref="D14:D19" si="0">SUM(E18:AI18)/20</f>
+        <f>SUM(E18:AI18)/20</f>
         <v>32.75</v>
       </c>
       <c r="E18" s="1">
@@ -1319,6 +2648,95 @@
       </c>
       <c r="R19" s="1">
         <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="2:24" x14ac:dyDescent="0.45">
+      <c r="C23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="2:24" x14ac:dyDescent="0.45">
+      <c r="B24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" s="1">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="2:24" x14ac:dyDescent="0.45">
+      <c r="B25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="2:24" x14ac:dyDescent="0.45">
+      <c r="B26" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" s="1">
+        <v>63</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="2:24" x14ac:dyDescent="0.45">
+      <c r="B27" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D27" s="1">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="2:24" x14ac:dyDescent="0.45">
+      <c r="B28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" s="1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="2:24" x14ac:dyDescent="0.45">
+      <c r="B29" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D29" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="2:24" x14ac:dyDescent="0.45">
+      <c r="B30" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="1">
+        <v>48</v>
+      </c>
+      <c r="D30" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="2:24" x14ac:dyDescent="0.45">
+      <c r="B31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C31" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="2:24" x14ac:dyDescent="0.45">
+      <c r="B32" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C32" s="1">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1327,5 +2745,115 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:C20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B3" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B5" s="3"/>
+      <c r="C5" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B6" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B7" s="5"/>
+      <c r="C7" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B10" s="3"/>
+      <c r="C10" s="17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B11" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B12" s="9"/>
+      <c r="C12" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B13" s="5"/>
+      <c r="C13" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B18" s="3"/>
+      <c r="C18" s="17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B19" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B20" s="5"/>
+      <c r="C20" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ressources pour le poster
</commit_message>
<xml_diff>
--- a/Tests.xlsx
+++ b/Tests.xlsx
@@ -9,14 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="11078"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="11078" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="5x5" sheetId="1" r:id="rId1"/>
-    <sheet name="6x6" sheetId="2" r:id="rId2"/>
+    <sheet name="7x7" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -111,12 +110,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="12">
@@ -258,7 +263,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -323,6 +328,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -714,11 +722,11 @@
           </c:downBars>
         </c:upDownBars>
         <c:smooth val="0"/>
-        <c:axId val="-1863244864"/>
-        <c:axId val="-1863250848"/>
+        <c:axId val="357524000"/>
+        <c:axId val="357524544"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1863244864"/>
+        <c:axId val="357524000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -824,7 +832,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1863250848"/>
+        <c:crossAx val="357524544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -832,7 +840,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1863250848"/>
+        <c:axId val="357524544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="80"/>
@@ -952,7 +960,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1863244864"/>
+        <c:crossAx val="357524000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="20"/>
@@ -1911,7 +1919,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
@@ -2753,8 +2761,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:C20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2773,7 +2781,7 @@
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B5" s="3"/>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="24" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>